<commit_message>
Changed argument sources in command table
</commit_message>
<xml_diff>
--- a/questions/Assignment 6 - Blue Gecko Client Command Table.xlsx
+++ b/questions/Assignment 6 - Blue Gecko Client Command Table.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="100">
   <si>
     <t>Event Handler Event</t>
   </si>
@@ -181,6 +181,9 @@
     <t>connection, service, uuid len, uuid data</t>
   </si>
   <si>
+    <t>service from evt_gatt_service, rest const values</t>
+  </si>
+  <si>
     <t>"Characteristics Discovered"</t>
   </si>
   <si>
@@ -203,6 +206,9 @@
   </si>
   <si>
     <t>connection, characteristics, flags</t>
+  </si>
+  <si>
+    <t>from evt_gatt_characteristic</t>
   </si>
   <si>
     <t>"Notifications Enabled"</t>
@@ -912,17 +918,17 @@
       <c r="F8" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="22" t="s">
-        <v>42</v>
+      <c r="G8" s="18" t="s">
+        <v>56</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="I8" s="21" t="s">
         <v>46</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K8" s="29" t="s">
         <v>39</v>
@@ -931,10 +937,10 @@
         <v>48</v>
       </c>
       <c r="M8" s="21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N8" s="25" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
@@ -961,34 +967,34 @@
     </row>
     <row r="9">
       <c r="A9" s="28" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D9" s="28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>42</v>
+        <v>64</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="H9" s="18" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K9" s="29" t="s">
         <v>53</v>
@@ -997,10 +1003,10 @@
         <v>48</v>
       </c>
       <c r="M9" s="21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="N9" s="25" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
@@ -1027,31 +1033,31 @@
     </row>
     <row r="10">
       <c r="A10" s="16" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G10" s="22" t="s">
         <v>42</v>
       </c>
       <c r="H10" s="16" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I10" s="21" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="J10" s="30" t="s">
         <v>48</v>
@@ -1063,10 +1069,10 @@
         <v>48</v>
       </c>
       <c r="M10" s="21" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="N10" s="25" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O10" s="8"/>
       <c r="P10" s="8"/>
@@ -1093,10 +1099,10 @@
     </row>
     <row r="11">
       <c r="A11" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>16</v>
@@ -1159,10 +1165,10 @@
     </row>
     <row r="12">
       <c r="A12" s="6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C12" s="13" t="s">
         <v>19</v>
@@ -1225,10 +1231,10 @@
     </row>
     <row r="13">
       <c r="A13" s="6" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>16</v>
@@ -1315,7 +1321,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1333,22 +1339,22 @@
     </row>
     <row r="17">
       <c r="A17" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G17" s="8" t="s">
         <v>42</v>
@@ -1370,42 +1376,42 @@
         <v>18</v>
       </c>
       <c r="N17" s="12" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="6" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G18" s="8" t="s">
         <v>42</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>18</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="L18" s="8" t="s">
         <v>18</v>
@@ -1414,7 +1420,7 @@
         <v>18</v>
       </c>
       <c r="N18" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19">
@@ -1435,7 +1441,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="8"/>
@@ -1453,28 +1459,28 @@
     </row>
     <row r="21">
       <c r="A21" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>42</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>18</v>
@@ -1492,7 +1498,7 @@
         <v>18</v>
       </c>
       <c r="N21" s="12" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22">

</xml_diff>